<commit_message>
add results to excel file on asymmetric uncertainty
</commit_message>
<xml_diff>
--- a/WA WB 4 to 12.xlsx
+++ b/WA WB 4 to 12.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristy\Documents\GitHub\political-uncertainty\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>al</t>
   </si>
@@ -71,12 +75,18 @@
   <si>
     <t>ValA</t>
   </si>
+  <si>
+    <t>sy=1.1</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,8 +113,21 @@
       <name val="Lucida Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF555555"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,8 +152,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0F0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -158,11 +187,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -198,6 +255,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -207,6 +273,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -255,7 +324,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -290,7 +359,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -501,15 +570,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A70" activePane="bottomLeft"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="600" topLeftCell="A40" activePane="bottomLeft"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="M87" sqref="M87"/>
+      <selection pane="bottomLeft" activeCell="V43" sqref="V43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="15.75" thickBot="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,7 +634,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="15.75" thickBot="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -624,7 +693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="15.75" thickBot="1">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -683,7 +752,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="15.75" thickBot="1">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -742,7 +811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="15.75" thickBot="1">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -801,7 +870,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="15.75" thickBot="1">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -860,7 +929,7 @@
         <v>4.0184300000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="15.75" thickBot="1">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -919,7 +988,7 @@
         <v>4.6454089999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="15.75" thickBot="1">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -978,7 +1047,7 @@
         <v>5.3474870000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="15.75" thickBot="1">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1037,7 +1106,7 @@
         <v>6.0936870000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="15.75" thickBot="1">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1096,7 +1165,7 @@
         <v>6.8726940000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="15.75" thickBot="1">
       <c r="A13" s="2">
         <v>1</v>
       </c>
@@ -1155,7 +1224,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="15.75" thickBot="1">
       <c r="A14" s="2">
         <v>2</v>
       </c>
@@ -1214,7 +1283,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="15.75" thickBot="1">
       <c r="A15" s="2">
         <v>3</v>
       </c>
@@ -1273,7 +1342,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="15.75" thickBot="1">
       <c r="A16" s="2">
         <v>4</v>
       </c>
@@ -1332,7 +1401,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="15.75" thickBot="1">
       <c r="A17" s="2">
         <v>5</v>
       </c>
@@ -1391,7 +1460,7 @@
         <v>4.0184300000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="15.75" thickBot="1">
       <c r="A18" s="2">
         <v>6</v>
       </c>
@@ -1450,7 +1519,7 @@
         <v>4.6454089999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="15.75" thickBot="1">
       <c r="A19" s="2">
         <v>7</v>
       </c>
@@ -1509,7 +1578,7 @@
         <v>5.3474870000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="15.75" thickBot="1">
       <c r="A20" s="2">
         <v>8</v>
       </c>
@@ -1568,7 +1637,7 @@
         <v>6.0936870000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="15.75" thickBot="1">
       <c r="A21" s="2">
         <v>9</v>
       </c>
@@ -1627,7 +1696,7 @@
         <v>6.8726940000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="15.75" thickBot="1">
       <c r="A23" s="2">
         <v>1</v>
       </c>
@@ -1686,7 +1755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="15.75" thickBot="1">
       <c r="A24" s="2">
         <v>2</v>
       </c>
@@ -1745,7 +1814,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="15.75" thickBot="1">
       <c r="A25" s="2">
         <v>3</v>
       </c>
@@ -1804,7 +1873,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="15.75" thickBot="1">
       <c r="A26" s="2">
         <v>4</v>
       </c>
@@ -1863,7 +1932,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="2">
         <v>5</v>
       </c>
@@ -1922,7 +1991,7 @@
         <v>4.0184300000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="15.75" thickBot="1">
       <c r="A28" s="2">
         <v>6</v>
       </c>
@@ -1981,7 +2050,7 @@
         <v>4.6454089999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="15.75" thickBot="1">
       <c r="A29" s="2">
         <v>7</v>
       </c>
@@ -2040,7 +2109,7 @@
         <v>5.3474870000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="15.75" thickBot="1">
       <c r="A30" s="2">
         <v>8</v>
       </c>
@@ -2099,7 +2168,7 @@
         <v>6.0936870000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="15.75" thickBot="1">
       <c r="A31" s="2">
         <v>9</v>
       </c>
@@ -2158,7 +2227,7 @@
         <v>6.8726940000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="15.75" thickBot="1">
       <c r="A33" s="2">
         <v>1</v>
       </c>
@@ -2217,7 +2286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="15.75" thickBot="1">
       <c r="A34" s="2">
         <v>2</v>
       </c>
@@ -2276,7 +2345,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="15.75" thickBot="1">
       <c r="A35" s="2">
         <v>3</v>
       </c>
@@ -2335,7 +2404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="15.75" thickBot="1">
       <c r="A36" s="2">
         <v>4</v>
       </c>
@@ -2394,7 +2463,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="15.75" thickBot="1">
       <c r="A37" s="2">
         <v>5</v>
       </c>
@@ -2453,7 +2522,7 @@
         <v>4.0184300000000004</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" ht="15.75" thickBot="1">
       <c r="A38" s="2">
         <v>6</v>
       </c>
@@ -2512,7 +2581,7 @@
         <v>4.6454089999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="15.75" thickBot="1">
       <c r="A39" s="2">
         <v>7</v>
       </c>
@@ -2571,7 +2640,7 @@
         <v>5.3474870000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="15.75" thickBot="1">
       <c r="A40" s="2">
         <v>8</v>
       </c>
@@ -2630,7 +2699,7 @@
         <v>6.0936870000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="15.75" thickBot="1">
       <c r="A41" s="2">
         <v>9</v>
       </c>
@@ -2689,7 +2758,7 @@
         <v>6.8726940000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="15.75" thickBot="1">
       <c r="A43" s="2">
         <v>1</v>
       </c>
@@ -2748,7 +2817,7 @@
         <v>1.747876</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="15.75" thickBot="1">
       <c r="A44" s="2">
         <v>2</v>
       </c>
@@ -2807,7 +2876,7 @@
         <v>2.1848459999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="15.75" thickBot="1">
       <c r="A45" s="2">
         <v>3</v>
       </c>
@@ -2866,7 +2935,7 @@
         <v>2.734756</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" ht="15.75" thickBot="1">
       <c r="A46" s="2">
         <v>4</v>
       </c>
@@ -2925,7 +2994,7 @@
         <v>3.3572150000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" ht="15.75" thickBot="1">
       <c r="A47" s="2">
         <v>5</v>
       </c>
@@ -2984,7 +3053,7 @@
         <v>3.9796749999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" ht="15.75" thickBot="1">
       <c r="A48" s="2">
         <v>6</v>
       </c>
@@ -3043,7 +3112,7 @@
         <v>4.6182699999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" ht="15.75" thickBot="1">
       <c r="A49" s="2">
         <v>7</v>
       </c>
@@ -3102,7 +3171,7 @@
         <v>5.3248530000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" ht="15.75" thickBot="1">
       <c r="A50" s="2">
         <v>8</v>
       </c>
@@ -3161,7 +3230,7 @@
         <v>6.0818320000000003</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" ht="15.75" thickBot="1">
       <c r="A51" s="2">
         <v>9</v>
       </c>
@@ -3220,7 +3289,7 @@
         <v>6.8709769999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" ht="15.75" thickBot="1">
       <c r="A53" s="2">
         <v>1</v>
       </c>
@@ -3279,7 +3348,7 @@
         <v>1.2941149999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" ht="15.75" thickBot="1">
       <c r="A54" s="2">
         <v>2</v>
       </c>
@@ -3338,7 +3407,7 @@
         <v>1.6176440000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" ht="15.75" thickBot="1">
       <c r="A55" s="2">
         <v>3</v>
       </c>
@@ -3397,7 +3466,7 @@
         <v>1.9411719999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" ht="15.75" thickBot="1">
       <c r="A56" s="2">
         <v>4</v>
       </c>
@@ -3456,7 +3525,7 @@
         <v>2.2647010000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" ht="15.75" thickBot="1">
       <c r="A57" s="2">
         <v>5</v>
       </c>
@@ -3515,7 +3584,7 @@
         <v>2.9807299999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" ht="15.75" thickBot="1">
       <c r="A58" s="2">
         <v>6</v>
       </c>
@@ -3574,7 +3643,7 @@
         <v>3.8783219999999998</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" ht="15.75" thickBot="1">
       <c r="A59" s="2">
         <v>7</v>
       </c>
@@ -3633,7 +3702,7 @@
         <v>4.7759130000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" ht="15.75" thickBot="1">
       <c r="A60" s="2">
         <v>8</v>
       </c>
@@ -3692,7 +3761,7 @@
         <v>5.6735040000000003</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" ht="15.75" thickBot="1">
       <c r="A61" s="2">
         <v>9</v>
       </c>
@@ -3751,7 +3820,7 @@
         <v>6.5710949999999997</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" ht="15.75" thickBot="1">
       <c r="A63" s="2">
         <v>1</v>
       </c>
@@ -3810,7 +3879,7 @@
         <v>1.059874</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" ht="15.75" thickBot="1">
       <c r="A64" s="2">
         <v>2</v>
       </c>
@@ -3869,7 +3938,7 @@
         <v>1.324843</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" ht="15.75" thickBot="1">
       <c r="A65" s="2">
         <v>3</v>
       </c>
@@ -3928,7 +3997,7 @@
         <v>1.5898110000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" ht="15.75" thickBot="1">
       <c r="A66" s="2">
         <v>4</v>
       </c>
@@ -3987,7 +4056,7 @@
         <v>1.8547800000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" ht="15.75" thickBot="1">
       <c r="A67" s="2">
         <v>5</v>
       </c>
@@ -4046,7 +4115,7 @@
         <v>2.4453990000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" ht="15.75" thickBot="1">
       <c r="A68" s="2">
         <v>6</v>
       </c>
@@ -4105,7 +4174,7 @@
         <v>3.376074</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" ht="15.75" thickBot="1">
       <c r="A69" s="2">
         <v>7</v>
       </c>
@@ -4164,7 +4233,7 @@
         <v>4.3067489999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" ht="15.75" thickBot="1">
       <c r="A70" s="2">
         <v>8</v>
       </c>
@@ -4223,7 +4292,7 @@
         <v>5.2374239999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" ht="15.75" thickBot="1">
       <c r="A71" s="2">
         <v>9</v>
       </c>
@@ -4282,7 +4351,7 @@
         <v>6.1680989999999998</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:19" ht="15.75" thickBot="1">
       <c r="A73" s="2">
         <v>1</v>
       </c>
@@ -4341,7 +4410,7 @@
         <v>0.90515330000000005</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:19" ht="15.75" thickBot="1">
       <c r="A74" s="2">
         <v>2</v>
       </c>
@@ -4400,7 +4469,7 @@
         <v>1.1314416</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" ht="15.75" thickBot="1">
       <c r="A75" s="2">
         <v>3</v>
       </c>
@@ -4459,7 +4528,7 @@
         <v>1.3577299</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:19" ht="15.75" thickBot="1">
       <c r="A76" s="2">
         <v>4</v>
       </c>
@@ -4518,7 +4587,7 @@
         <v>1.5840182</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:19" ht="15.75" thickBot="1">
       <c r="A77" s="2">
         <v>5</v>
       </c>
@@ -4577,7 +4646,7 @@
         <v>2.0076984000000002</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:19" ht="15.75" thickBot="1">
       <c r="A78" s="2">
         <v>6</v>
       </c>
@@ -4636,7 +4705,7 @@
         <v>2.9586606999999998</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:19" ht="15.75" thickBot="1">
       <c r="A79" s="2">
         <v>7</v>
       </c>
@@ -4695,7 +4764,7 @@
         <v>3.9096229999999998</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:19" ht="15.75" thickBot="1">
       <c r="A80" s="2">
         <v>8</v>
       </c>
@@ -4754,7 +4823,7 @@
         <v>4.8605853000000003</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:19" ht="15.75" thickBot="1">
       <c r="A81" s="2">
         <v>9</v>
       </c>
@@ -4813,7 +4882,7 @@
         <v>5.8115477000000002</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19">
       <c r="A83" s="12"/>
       <c r="B83" s="12"/>
       <c r="C83" s="12"/>
@@ -4834,7 +4903,7 @@
       <c r="R83" s="12"/>
       <c r="S83" s="7"/>
     </row>
-    <row r="84" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:19" ht="15.75" thickBot="1">
       <c r="A84" s="2">
         <v>1</v>
       </c>
@@ -4893,7 +4962,7 @@
         <v>0.79329360000000004</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:19" ht="15.75" thickBot="1">
       <c r="A85" s="2">
         <v>2</v>
       </c>
@@ -4952,7 +5021,7 @@
         <v>0.99161699999999997</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:19" ht="15.75" thickBot="1">
       <c r="A86" s="2">
         <v>3</v>
       </c>
@@ -5011,7 +5080,7 @@
         <v>1.1899403</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:19" ht="15.75" thickBot="1">
       <c r="A87" s="2">
         <v>4</v>
       </c>
@@ -5070,7 +5139,7 @@
         <v>1.3882637</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:19" ht="15.75" thickBot="1">
       <c r="A88" s="2">
         <v>5</v>
       </c>
@@ -5129,7 +5198,7 @@
         <v>1.8487115999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:19" ht="15.75" thickBot="1">
       <c r="A89" s="2">
         <v>6</v>
       </c>
@@ -5188,7 +5257,7 @@
         <v>2.8048004999999998</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:19" ht="15.75" thickBot="1">
       <c r="A90" s="2">
         <v>7</v>
       </c>
@@ -5247,7 +5316,7 @@
         <v>3.7608895000000002</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:19" ht="15.75" thickBot="1">
       <c r="A91" s="2">
         <v>8</v>
       </c>
@@ -5306,7 +5375,7 @@
         <v>4.7169784000000003</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:19" ht="15.75" thickBot="1">
       <c r="A92" s="2">
         <v>9</v>
       </c>
@@ -5373,24 +5442,1139 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A2" s="13"/>
+      <c r="B2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15">
+        <v>8</v>
+      </c>
+      <c r="E3" s="15">
+        <v>0</v>
+      </c>
+      <c r="F3" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="G3" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="15">
+        <v>0</v>
+      </c>
+      <c r="I3" s="15">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="J3" s="15">
+        <v>0</v>
+      </c>
+      <c r="K3" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="L3" s="15">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="M3" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="N3" s="15">
+        <v>3.9738370000000001</v>
+      </c>
+      <c r="O3" s="15">
+        <v>0.55472960000000004</v>
+      </c>
+      <c r="P3" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="15">
+        <v>0</v>
+      </c>
+      <c r="R3" s="15">
+        <v>0</v>
+      </c>
+      <c r="S3" s="15">
+        <v>1.7810809999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A4" s="13">
+        <v>2</v>
+      </c>
+      <c r="B4" s="15">
+        <v>0</v>
+      </c>
+      <c r="C4" s="15">
+        <v>5</v>
+      </c>
+      <c r="D4" s="15">
+        <v>8</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0</v>
+      </c>
+      <c r="F4" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="G4" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="15">
+        <v>0</v>
+      </c>
+      <c r="I4" s="15">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="J4" s="15">
+        <v>0</v>
+      </c>
+      <c r="K4" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="L4" s="15">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="M4" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="N4" s="15">
+        <v>3.9738370000000001</v>
+      </c>
+      <c r="O4" s="15">
+        <v>0.55472960000000004</v>
+      </c>
+      <c r="P4" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="15">
+        <v>0</v>
+      </c>
+      <c r="R4" s="15">
+        <v>0</v>
+      </c>
+      <c r="S4" s="15">
+        <v>2.2263519999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A5" s="13">
+        <v>3</v>
+      </c>
+      <c r="B5" s="15">
+        <v>0</v>
+      </c>
+      <c r="C5" s="15">
+        <v>6</v>
+      </c>
+      <c r="D5" s="15">
+        <v>8</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0</v>
+      </c>
+      <c r="F5" s="15">
+        <v>-0.1</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="15">
+        <v>0</v>
+      </c>
+      <c r="I5" s="15">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="J5" s="15">
+        <v>0</v>
+      </c>
+      <c r="K5" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="L5" s="15">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="M5" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="N5" s="15">
+        <v>3.6025689999999999</v>
+      </c>
+      <c r="O5" s="15">
+        <v>0.47669610000000001</v>
+      </c>
+      <c r="P5" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="R5" s="15">
+        <v>0</v>
+      </c>
+      <c r="S5" s="15">
+        <v>2.739824</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A6" s="13">
+        <v>4</v>
+      </c>
+      <c r="B6" s="15">
+        <v>0</v>
+      </c>
+      <c r="C6" s="15">
+        <v>7</v>
+      </c>
+      <c r="D6" s="15">
+        <v>8</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0</v>
+      </c>
+      <c r="F6" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="G6" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="H6" s="15">
+        <v>0</v>
+      </c>
+      <c r="I6" s="15">
+        <v>0</v>
+      </c>
+      <c r="J6" s="15">
+        <v>0</v>
+      </c>
+      <c r="K6" s="15">
+        <v>-0.9</v>
+      </c>
+      <c r="L6" s="15">
+        <v>0</v>
+      </c>
+      <c r="M6" s="15">
+        <v>-0.1</v>
+      </c>
+      <c r="N6" s="15">
+        <v>3.0653549999999998</v>
+      </c>
+      <c r="O6" s="15">
+        <v>0.38316939999999999</v>
+      </c>
+      <c r="P6" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="R6" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="S6" s="15">
+        <v>3.3178139999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A7" s="13">
+        <v>5</v>
+      </c>
+      <c r="B7" s="15">
+        <v>0</v>
+      </c>
+      <c r="C7" s="15">
+        <v>8</v>
+      </c>
+      <c r="D7" s="15">
+        <v>8</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0</v>
+      </c>
+      <c r="F7" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="G7" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="H7" s="15">
+        <v>0</v>
+      </c>
+      <c r="I7" s="15">
+        <v>0</v>
+      </c>
+      <c r="J7" s="15">
+        <v>0</v>
+      </c>
+      <c r="K7" s="15">
+        <v>-0.9</v>
+      </c>
+      <c r="L7" s="15">
+        <v>0</v>
+      </c>
+      <c r="M7" s="15">
+        <v>-0.1</v>
+      </c>
+      <c r="N7" s="15">
+        <v>3.0653549999999998</v>
+      </c>
+      <c r="O7" s="15">
+        <v>0.38316939999999999</v>
+      </c>
+      <c r="P7" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="R7" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="S7" s="15">
+        <v>3.9346450000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A8" s="13">
+        <v>6</v>
+      </c>
+      <c r="B8" s="15">
+        <v>0</v>
+      </c>
+      <c r="C8" s="15">
+        <v>9</v>
+      </c>
+      <c r="D8" s="15">
+        <v>8</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="F8" s="15">
+        <v>-0.1</v>
+      </c>
+      <c r="G8" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="H8" s="15">
+        <v>0</v>
+      </c>
+      <c r="I8" s="15">
+        <v>0</v>
+      </c>
+      <c r="J8" s="15">
+        <v>0</v>
+      </c>
+      <c r="K8" s="15">
+        <v>-0.9</v>
+      </c>
+      <c r="L8" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="M8" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="N8" s="15">
+        <v>2.472588</v>
+      </c>
+      <c r="O8" s="15">
+        <v>0.3090735</v>
+      </c>
+      <c r="P8" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="Q8" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="R8" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="S8" s="15">
+        <v>4.6183389999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A9" s="13">
+        <v>7</v>
+      </c>
+      <c r="B9" s="15">
+        <v>0</v>
+      </c>
+      <c r="C9" s="15">
+        <v>10</v>
+      </c>
+      <c r="D9" s="15">
+        <v>8</v>
+      </c>
+      <c r="E9" s="15">
+        <v>1</v>
+      </c>
+      <c r="F9" s="15">
+        <v>-0.1</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="H9" s="15">
+        <v>0</v>
+      </c>
+      <c r="I9" s="15">
+        <v>0</v>
+      </c>
+      <c r="J9" s="15">
+        <v>0</v>
+      </c>
+      <c r="K9" s="15">
+        <v>-0.9</v>
+      </c>
+      <c r="L9" s="15">
+        <v>-1</v>
+      </c>
+      <c r="M9" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="N9" s="15">
+        <v>2.3051020000000002</v>
+      </c>
+      <c r="O9" s="15">
+        <v>0.2881378</v>
+      </c>
+      <c r="P9" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="R9" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="S9" s="15">
+        <v>5.3186220000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A10" s="13">
+        <v>8</v>
+      </c>
+      <c r="B10" s="15">
+        <v>0</v>
+      </c>
+      <c r="C10" s="15">
+        <v>11</v>
+      </c>
+      <c r="D10" s="15">
+        <v>8</v>
+      </c>
+      <c r="E10" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="F10" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="G10" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H10" s="15">
+        <v>0</v>
+      </c>
+      <c r="I10" s="15">
+        <v>0</v>
+      </c>
+      <c r="J10" s="15">
+        <v>0</v>
+      </c>
+      <c r="K10" s="15">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="L10" s="15">
+        <v>-1.2</v>
+      </c>
+      <c r="M10" s="15">
+        <v>-0.1</v>
+      </c>
+      <c r="N10" s="15">
+        <v>1.8584339999999999</v>
+      </c>
+      <c r="O10" s="15">
+        <v>0.23230419999999999</v>
+      </c>
+      <c r="P10" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="Q10" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="R10" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="S10" s="15">
+        <v>6.0446530000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A11" s="13">
+        <v>9</v>
+      </c>
+      <c r="B11" s="15">
+        <v>0</v>
+      </c>
+      <c r="C11" s="15">
+        <v>12</v>
+      </c>
+      <c r="D11" s="15">
+        <v>8</v>
+      </c>
+      <c r="E11" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="F11" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="G11" s="15">
+        <v>1.3</v>
+      </c>
+      <c r="H11" s="15">
+        <v>0</v>
+      </c>
+      <c r="I11" s="15">
+        <v>0</v>
+      </c>
+      <c r="J11" s="15">
+        <v>0</v>
+      </c>
+      <c r="K11" s="15">
+        <v>-1.3</v>
+      </c>
+      <c r="L11" s="15">
+        <v>-1.2</v>
+      </c>
+      <c r="M11" s="15">
+        <v>-0.1</v>
+      </c>
+      <c r="N11" s="15">
+        <v>1.719606</v>
+      </c>
+      <c r="O11" s="15">
+        <v>0.21495069999999999</v>
+      </c>
+      <c r="P11" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="Q11" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="R11" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="S11" s="15">
+        <v>6.8205920000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>-0.5</v>
+      </c>
+      <c r="G13">
+        <v>0.5</v>
+      </c>
+      <c r="H13">
+        <v>1.2549999999999999</v>
+      </c>
+      <c r="I13">
+        <v>0.755</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0.755</v>
+      </c>
+      <c r="L13">
+        <v>0.755</v>
+      </c>
+      <c r="M13">
+        <v>0.5</v>
+      </c>
+      <c r="N13">
+        <v>5.2786597999999998</v>
+      </c>
+      <c r="O13">
+        <v>0.72886598000000002</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>1.0845359999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>-0.5</v>
+      </c>
+      <c r="G14">
+        <v>0.5</v>
+      </c>
+      <c r="H14">
+        <v>1.2549999999999999</v>
+      </c>
+      <c r="I14">
+        <v>0.755</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0.755</v>
+      </c>
+      <c r="L14">
+        <v>0.755</v>
+      </c>
+      <c r="M14">
+        <v>0.5</v>
+      </c>
+      <c r="N14">
+        <v>5.2786597999999998</v>
+      </c>
+      <c r="O14">
+        <v>0.72886598000000002</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>1.3556699999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>-0.5</v>
+      </c>
+      <c r="G15">
+        <v>0.5</v>
+      </c>
+      <c r="H15">
+        <v>1.2549999999999999</v>
+      </c>
+      <c r="I15">
+        <v>0.755</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0.755</v>
+      </c>
+      <c r="L15">
+        <v>0.755</v>
+      </c>
+      <c r="M15">
+        <v>0.5</v>
+      </c>
+      <c r="N15">
+        <v>5.2786597999999998</v>
+      </c>
+      <c r="O15">
+        <v>0.72886598000000002</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>1.6268039999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>-0.5</v>
+      </c>
+      <c r="G16">
+        <v>0.5</v>
+      </c>
+      <c r="H16">
+        <v>1.2549999999999999</v>
+      </c>
+      <c r="I16">
+        <v>0.755</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0.755</v>
+      </c>
+      <c r="L16">
+        <v>0.755</v>
+      </c>
+      <c r="M16">
+        <v>0.5</v>
+      </c>
+      <c r="N16">
+        <v>5.2786597999999998</v>
+      </c>
+      <c r="O16">
+        <v>0.72886598000000002</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>1.8979379999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>1.8</v>
+      </c>
+      <c r="F17">
+        <v>1.5</v>
+      </c>
+      <c r="G17">
+        <v>1.7</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>-1.7</v>
+      </c>
+      <c r="L17">
+        <v>-1.8</v>
+      </c>
+      <c r="M17">
+        <v>-1.5</v>
+      </c>
+      <c r="N17">
+        <v>0.73331489999999999</v>
+      </c>
+      <c r="O17">
+        <v>7.3331489999999999E-2</v>
+      </c>
+      <c r="P17">
+        <v>1.8</v>
+      </c>
+      <c r="Q17">
+        <v>2</v>
+      </c>
+      <c r="R17">
+        <v>1.2</v>
+      </c>
+      <c r="S17">
+        <v>2.413348</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <v>1.8</v>
+      </c>
+      <c r="F18">
+        <v>1.5</v>
+      </c>
+      <c r="G18">
+        <v>1.7</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>-1.7</v>
+      </c>
+      <c r="L18">
+        <v>-1.8</v>
+      </c>
+      <c r="M18">
+        <v>-1.5</v>
+      </c>
+      <c r="N18">
+        <v>0.73331489999999999</v>
+      </c>
+      <c r="O18">
+        <v>7.3331489999999999E-2</v>
+      </c>
+      <c r="P18">
+        <v>1.8</v>
+      </c>
+      <c r="Q18">
+        <v>2</v>
+      </c>
+      <c r="R18">
+        <v>1.2</v>
+      </c>
+      <c r="S18">
+        <v>3.340017</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <v>1.8</v>
+      </c>
+      <c r="F19">
+        <v>1.5</v>
+      </c>
+      <c r="G19">
+        <v>1.7</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>-1.7</v>
+      </c>
+      <c r="L19">
+        <v>-1.8</v>
+      </c>
+      <c r="M19">
+        <v>-1.5</v>
+      </c>
+      <c r="N19">
+        <v>0.73331489999999999</v>
+      </c>
+      <c r="O19">
+        <v>7.3331489999999999E-2</v>
+      </c>
+      <c r="P19">
+        <v>1.8</v>
+      </c>
+      <c r="Q19">
+        <v>2</v>
+      </c>
+      <c r="R19">
+        <v>1.2</v>
+      </c>
+      <c r="S19">
+        <v>4.2666849999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>11</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <v>1.8</v>
+      </c>
+      <c r="F20">
+        <v>1.5</v>
+      </c>
+      <c r="G20">
+        <v>1.7</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>-1.7</v>
+      </c>
+      <c r="L20">
+        <v>-1.8</v>
+      </c>
+      <c r="M20">
+        <v>-1.5</v>
+      </c>
+      <c r="N20">
+        <v>0.73331489999999999</v>
+      </c>
+      <c r="O20">
+        <v>7.3331489999999999E-2</v>
+      </c>
+      <c r="P20">
+        <v>1.8</v>
+      </c>
+      <c r="Q20">
+        <v>2</v>
+      </c>
+      <c r="R20">
+        <v>1.2</v>
+      </c>
+      <c r="S20">
+        <v>5.1933540000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>12</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>1.8</v>
+      </c>
+      <c r="F21">
+        <v>1.5</v>
+      </c>
+      <c r="G21">
+        <v>1.7</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>-1.7</v>
+      </c>
+      <c r="L21">
+        <v>-1.8</v>
+      </c>
+      <c r="M21">
+        <v>-1.5</v>
+      </c>
+      <c r="N21">
+        <v>0.73331489999999999</v>
+      </c>
+      <c r="O21">
+        <v>7.3331489999999999E-2</v>
+      </c>
+      <c r="P21">
+        <v>1.8</v>
+      </c>
+      <c r="Q21">
+        <v>2</v>
+      </c>
+      <c r="R21">
+        <v>1.2</v>
+      </c>
+      <c r="S21">
+        <v>6.1200219999999996</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add even more asymmetric results to excel file
</commit_message>
<xml_diff>
--- a/WA WB 4 to 12.xlsx
+++ b/WA WB 4 to 12.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
   <si>
     <t>al</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>sz</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -5451,10 +5454,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U131"/>
+  <dimension ref="A1:U191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121:U131"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="D180" sqref="D180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13201,6 +13204,3584 @@
         <v>3.7792849999999998</v>
       </c>
     </row>
+    <row r="132" spans="1:21" ht="15.75" thickBot="1"/>
+    <row r="133" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A133" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B133" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C133" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="D133" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="E133" s="15">
+        <v>5</v>
+      </c>
+      <c r="F133" s="15">
+        <v>8</v>
+      </c>
+      <c r="G133" s="15">
+        <v>1</v>
+      </c>
+      <c r="H133" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I133" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J133" s="15">
+        <v>0</v>
+      </c>
+      <c r="K133" s="15">
+        <v>0</v>
+      </c>
+      <c r="L133" s="15">
+        <v>0</v>
+      </c>
+      <c r="M133" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N133" s="15">
+        <v>-1.3</v>
+      </c>
+      <c r="O133" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="P133" s="15">
+        <v>2.3942700000000001</v>
+      </c>
+      <c r="Q133" s="15">
+        <v>0.29928369999999999</v>
+      </c>
+      <c r="R133" s="15">
+        <v>1</v>
+      </c>
+      <c r="S133" s="15">
+        <v>0</v>
+      </c>
+      <c r="T133" s="15">
+        <v>0</v>
+      </c>
+      <c r="U133" s="15">
+        <v>2.5035810000000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A134" s="13">
+        <v>2</v>
+      </c>
+      <c r="B134" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C134" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="D134" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="E134" s="15">
+        <v>5.4</v>
+      </c>
+      <c r="F134" s="15">
+        <v>8</v>
+      </c>
+      <c r="G134" s="15">
+        <v>1</v>
+      </c>
+      <c r="H134" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I134" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J134" s="15">
+        <v>0</v>
+      </c>
+      <c r="K134" s="15">
+        <v>0</v>
+      </c>
+      <c r="L134" s="15">
+        <v>0</v>
+      </c>
+      <c r="M134" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N134" s="15">
+        <v>-1.3</v>
+      </c>
+      <c r="O134" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="P134" s="15">
+        <v>2.3942700000000001</v>
+      </c>
+      <c r="Q134" s="15">
+        <v>0.29928369999999999</v>
+      </c>
+      <c r="R134" s="15">
+        <v>1</v>
+      </c>
+      <c r="S134" s="15">
+        <v>0</v>
+      </c>
+      <c r="T134" s="15">
+        <v>0</v>
+      </c>
+      <c r="U134" s="15">
+        <v>2.783868</v>
+      </c>
+    </row>
+    <row r="135" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A135" s="13">
+        <v>3</v>
+      </c>
+      <c r="B135" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C135" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="D135" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="E135" s="15">
+        <v>5.8</v>
+      </c>
+      <c r="F135" s="15">
+        <v>8</v>
+      </c>
+      <c r="G135" s="15">
+        <v>1</v>
+      </c>
+      <c r="H135" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I135" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J135" s="15">
+        <v>0</v>
+      </c>
+      <c r="K135" s="15">
+        <v>0</v>
+      </c>
+      <c r="L135" s="15">
+        <v>0</v>
+      </c>
+      <c r="M135" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N135" s="15">
+        <v>-1.3</v>
+      </c>
+      <c r="O135" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="P135" s="15">
+        <v>2.3942700000000001</v>
+      </c>
+      <c r="Q135" s="15">
+        <v>0.29928369999999999</v>
+      </c>
+      <c r="R135" s="15">
+        <v>1</v>
+      </c>
+      <c r="S135" s="15">
+        <v>0</v>
+      </c>
+      <c r="T135" s="15">
+        <v>0</v>
+      </c>
+      <c r="U135" s="15">
+        <v>3.0641539999999998</v>
+      </c>
+    </row>
+    <row r="136" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A136" s="13">
+        <v>4</v>
+      </c>
+      <c r="B136" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C136" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="D136" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="E136" s="15">
+        <v>6.2</v>
+      </c>
+      <c r="F136" s="15">
+        <v>8</v>
+      </c>
+      <c r="G136" s="15">
+        <v>1</v>
+      </c>
+      <c r="H136" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I136" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J136" s="15">
+        <v>0</v>
+      </c>
+      <c r="K136" s="15">
+        <v>0</v>
+      </c>
+      <c r="L136" s="15">
+        <v>0</v>
+      </c>
+      <c r="M136" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N136" s="15">
+        <v>-1.3</v>
+      </c>
+      <c r="O136" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="P136" s="15">
+        <v>2.3942700000000001</v>
+      </c>
+      <c r="Q136" s="15">
+        <v>0.29928369999999999</v>
+      </c>
+      <c r="R136" s="15">
+        <v>1</v>
+      </c>
+      <c r="S136" s="15">
+        <v>0</v>
+      </c>
+      <c r="T136" s="15">
+        <v>0</v>
+      </c>
+      <c r="U136" s="15">
+        <v>3.3444410000000002</v>
+      </c>
+    </row>
+    <row r="137" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A137" s="13">
+        <v>5</v>
+      </c>
+      <c r="B137" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C137" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="D137" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="E137" s="15">
+        <v>6.6</v>
+      </c>
+      <c r="F137" s="15">
+        <v>8</v>
+      </c>
+      <c r="G137" s="15">
+        <v>1</v>
+      </c>
+      <c r="H137" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I137" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J137" s="15">
+        <v>0</v>
+      </c>
+      <c r="K137" s="15">
+        <v>0</v>
+      </c>
+      <c r="L137" s="15">
+        <v>0</v>
+      </c>
+      <c r="M137" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N137" s="15">
+        <v>-1.3</v>
+      </c>
+      <c r="O137" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="P137" s="15">
+        <v>2.3942700000000001</v>
+      </c>
+      <c r="Q137" s="15">
+        <v>0.29928369999999999</v>
+      </c>
+      <c r="R137" s="15">
+        <v>1</v>
+      </c>
+      <c r="S137" s="15">
+        <v>0</v>
+      </c>
+      <c r="T137" s="15">
+        <v>0</v>
+      </c>
+      <c r="U137" s="15">
+        <v>3.624727</v>
+      </c>
+    </row>
+    <row r="138" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A138" s="13">
+        <v>6</v>
+      </c>
+      <c r="B138" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C138" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="D138" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="E138" s="15">
+        <v>7</v>
+      </c>
+      <c r="F138" s="15">
+        <v>8</v>
+      </c>
+      <c r="G138" s="15">
+        <v>1</v>
+      </c>
+      <c r="H138" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I138" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J138" s="15">
+        <v>0</v>
+      </c>
+      <c r="K138" s="15">
+        <v>0</v>
+      </c>
+      <c r="L138" s="15">
+        <v>0</v>
+      </c>
+      <c r="M138" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N138" s="15">
+        <v>-1.3</v>
+      </c>
+      <c r="O138" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="P138" s="15">
+        <v>2.3942700000000001</v>
+      </c>
+      <c r="Q138" s="15">
+        <v>0.29928369999999999</v>
+      </c>
+      <c r="R138" s="15">
+        <v>1</v>
+      </c>
+      <c r="S138" s="15">
+        <v>0</v>
+      </c>
+      <c r="T138" s="15">
+        <v>0</v>
+      </c>
+      <c r="U138" s="15">
+        <v>3.905014</v>
+      </c>
+    </row>
+    <row r="139" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A139" s="13">
+        <v>7</v>
+      </c>
+      <c r="B139" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C139" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="D139" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="E139" s="15">
+        <v>7.4</v>
+      </c>
+      <c r="F139" s="15">
+        <v>8</v>
+      </c>
+      <c r="G139" s="15">
+        <v>1</v>
+      </c>
+      <c r="H139" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I139" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J139" s="15">
+        <v>0</v>
+      </c>
+      <c r="K139" s="15">
+        <v>0</v>
+      </c>
+      <c r="L139" s="15">
+        <v>0</v>
+      </c>
+      <c r="M139" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N139" s="15">
+        <v>-1.3</v>
+      </c>
+      <c r="O139" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="P139" s="15">
+        <v>2.3942700000000001</v>
+      </c>
+      <c r="Q139" s="15">
+        <v>0.29928369999999999</v>
+      </c>
+      <c r="R139" s="15">
+        <v>1</v>
+      </c>
+      <c r="S139" s="15">
+        <v>0</v>
+      </c>
+      <c r="T139" s="15">
+        <v>0</v>
+      </c>
+      <c r="U139" s="15">
+        <v>4.1852999999999998</v>
+      </c>
+    </row>
+    <row r="140" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A140" s="13">
+        <v>8</v>
+      </c>
+      <c r="B140" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C140" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="D140" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="E140" s="15">
+        <v>7.8</v>
+      </c>
+      <c r="F140" s="15">
+        <v>8</v>
+      </c>
+      <c r="G140" s="15">
+        <v>1</v>
+      </c>
+      <c r="H140" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I140" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J140" s="15">
+        <v>0</v>
+      </c>
+      <c r="K140" s="15">
+        <v>0</v>
+      </c>
+      <c r="L140" s="15">
+        <v>0</v>
+      </c>
+      <c r="M140" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N140" s="15">
+        <v>-1.3</v>
+      </c>
+      <c r="O140" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="P140" s="15">
+        <v>2.3942700000000001</v>
+      </c>
+      <c r="Q140" s="15">
+        <v>0.29928369999999999</v>
+      </c>
+      <c r="R140" s="15">
+        <v>1</v>
+      </c>
+      <c r="S140" s="15">
+        <v>0</v>
+      </c>
+      <c r="T140" s="15">
+        <v>0</v>
+      </c>
+      <c r="U140" s="15">
+        <v>4.4655870000000002</v>
+      </c>
+    </row>
+    <row r="141" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A141" s="13">
+        <v>9</v>
+      </c>
+      <c r="B141" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C141" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="D141" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="E141" s="15">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F141" s="15">
+        <v>8</v>
+      </c>
+      <c r="G141" s="15">
+        <v>1</v>
+      </c>
+      <c r="H141" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I141" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J141" s="15">
+        <v>0</v>
+      </c>
+      <c r="K141" s="15">
+        <v>0</v>
+      </c>
+      <c r="L141" s="15">
+        <v>0</v>
+      </c>
+      <c r="M141" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N141" s="15">
+        <v>-1.3</v>
+      </c>
+      <c r="O141" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="P141" s="15">
+        <v>2.3942700000000001</v>
+      </c>
+      <c r="Q141" s="15">
+        <v>0.29928369999999999</v>
+      </c>
+      <c r="R141" s="15">
+        <v>1</v>
+      </c>
+      <c r="S141" s="15">
+        <v>0</v>
+      </c>
+      <c r="T141" s="15">
+        <v>0</v>
+      </c>
+      <c r="U141" s="15">
+        <v>4.7458729999999996</v>
+      </c>
+    </row>
+    <row r="142" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A142" s="13">
+        <v>10</v>
+      </c>
+      <c r="B142" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C142" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="D142" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="E142" s="15">
+        <v>8.6</v>
+      </c>
+      <c r="F142" s="15">
+        <v>8</v>
+      </c>
+      <c r="G142" s="15">
+        <v>1</v>
+      </c>
+      <c r="H142" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I142" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J142" s="15">
+        <v>0</v>
+      </c>
+      <c r="K142" s="15">
+        <v>0</v>
+      </c>
+      <c r="L142" s="15">
+        <v>0</v>
+      </c>
+      <c r="M142" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N142" s="15">
+        <v>-1.3</v>
+      </c>
+      <c r="O142" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="P142" s="15">
+        <v>2.3942700000000001</v>
+      </c>
+      <c r="Q142" s="15">
+        <v>0.29928369999999999</v>
+      </c>
+      <c r="R142" s="15">
+        <v>1</v>
+      </c>
+      <c r="S142" s="15">
+        <v>0</v>
+      </c>
+      <c r="T142" s="15">
+        <v>0</v>
+      </c>
+      <c r="U142" s="15">
+        <v>5.02616</v>
+      </c>
+    </row>
+    <row r="143" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A143" s="13">
+        <v>11</v>
+      </c>
+      <c r="B143" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C143" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="D143" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="E143" s="15">
+        <v>9</v>
+      </c>
+      <c r="F143" s="15">
+        <v>8</v>
+      </c>
+      <c r="G143" s="15">
+        <v>1</v>
+      </c>
+      <c r="H143" s="15">
+        <v>-0.1</v>
+      </c>
+      <c r="I143" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J143" s="15">
+        <v>0</v>
+      </c>
+      <c r="K143" s="15">
+        <v>0</v>
+      </c>
+      <c r="L143" s="15">
+        <v>0</v>
+      </c>
+      <c r="M143" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N143" s="15">
+        <v>-1.3</v>
+      </c>
+      <c r="O143" s="15">
+        <v>-0.2</v>
+      </c>
+      <c r="P143" s="15">
+        <v>2.0329989999999998</v>
+      </c>
+      <c r="Q143" s="15">
+        <v>0.25412489999999999</v>
+      </c>
+      <c r="R143" s="15">
+        <v>1</v>
+      </c>
+      <c r="S143" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="T143" s="15">
+        <v>0</v>
+      </c>
+      <c r="U143" s="15">
+        <v>5.3128760000000002</v>
+      </c>
+    </row>
+    <row r="144" spans="1:21" ht="15.75" thickBot="1"/>
+    <row r="145" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A145" s="13">
+        <v>1</v>
+      </c>
+      <c r="B145" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C145" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D145" s="15">
+        <v>1</v>
+      </c>
+      <c r="E145" s="15">
+        <v>5</v>
+      </c>
+      <c r="F145" s="15">
+        <v>8</v>
+      </c>
+      <c r="G145" s="15">
+        <v>0</v>
+      </c>
+      <c r="H145" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="I145" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J145" s="15">
+        <v>0</v>
+      </c>
+      <c r="K145" s="15">
+        <v>0</v>
+      </c>
+      <c r="L145" s="15">
+        <v>0</v>
+      </c>
+      <c r="M145" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N145" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="O145" s="15">
+        <v>0</v>
+      </c>
+      <c r="P145" s="15">
+        <v>2.9423319999999999</v>
+      </c>
+      <c r="Q145" s="15">
+        <v>0.36779149999999999</v>
+      </c>
+      <c r="R145" s="15">
+        <v>0</v>
+      </c>
+      <c r="S145" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="T145" s="15">
+        <v>0</v>
+      </c>
+      <c r="U145" s="15">
+        <v>2.961042</v>
+      </c>
+    </row>
+    <row r="146" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A146" s="13">
+        <v>2</v>
+      </c>
+      <c r="B146" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C146" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D146" s="15">
+        <v>1</v>
+      </c>
+      <c r="E146" s="15">
+        <v>5.4</v>
+      </c>
+      <c r="F146" s="15">
+        <v>8</v>
+      </c>
+      <c r="G146" s="15">
+        <v>0</v>
+      </c>
+      <c r="H146" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="I146" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J146" s="15">
+        <v>0</v>
+      </c>
+      <c r="K146" s="15">
+        <v>0</v>
+      </c>
+      <c r="L146" s="15">
+        <v>0</v>
+      </c>
+      <c r="M146" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N146" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="O146" s="15">
+        <v>0</v>
+      </c>
+      <c r="P146" s="15">
+        <v>2.9423319999999999</v>
+      </c>
+      <c r="Q146" s="15">
+        <v>0.36779149999999999</v>
+      </c>
+      <c r="R146" s="15">
+        <v>0</v>
+      </c>
+      <c r="S146" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="T146" s="15">
+        <v>0</v>
+      </c>
+      <c r="U146" s="15">
+        <v>3.2139259999999998</v>
+      </c>
+    </row>
+    <row r="147" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A147" s="13">
+        <v>3</v>
+      </c>
+      <c r="B147" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C147" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D147" s="15">
+        <v>1</v>
+      </c>
+      <c r="E147" s="15">
+        <v>5.8</v>
+      </c>
+      <c r="F147" s="15">
+        <v>8</v>
+      </c>
+      <c r="G147" s="15">
+        <v>0</v>
+      </c>
+      <c r="H147" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="I147" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J147" s="15">
+        <v>0</v>
+      </c>
+      <c r="K147" s="15">
+        <v>0</v>
+      </c>
+      <c r="L147" s="15">
+        <v>0</v>
+      </c>
+      <c r="M147" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N147" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="O147" s="15">
+        <v>0</v>
+      </c>
+      <c r="P147" s="15">
+        <v>2.9423319999999999</v>
+      </c>
+      <c r="Q147" s="15">
+        <v>0.36779149999999999</v>
+      </c>
+      <c r="R147" s="15">
+        <v>0</v>
+      </c>
+      <c r="S147" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="T147" s="15">
+        <v>0</v>
+      </c>
+      <c r="U147" s="15">
+        <v>3.466809</v>
+      </c>
+    </row>
+    <row r="148" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A148" s="13">
+        <v>4</v>
+      </c>
+      <c r="B148" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C148" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D148" s="15">
+        <v>1</v>
+      </c>
+      <c r="E148" s="15">
+        <v>6.2</v>
+      </c>
+      <c r="F148" s="15">
+        <v>8</v>
+      </c>
+      <c r="G148" s="15">
+        <v>0</v>
+      </c>
+      <c r="H148" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="I148" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J148" s="15">
+        <v>0</v>
+      </c>
+      <c r="K148" s="15">
+        <v>0</v>
+      </c>
+      <c r="L148" s="15">
+        <v>0</v>
+      </c>
+      <c r="M148" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N148" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="O148" s="15">
+        <v>0</v>
+      </c>
+      <c r="P148" s="15">
+        <v>2.9423319999999999</v>
+      </c>
+      <c r="Q148" s="15">
+        <v>0.36779149999999999</v>
+      </c>
+      <c r="R148" s="15">
+        <v>0</v>
+      </c>
+      <c r="S148" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="T148" s="15">
+        <v>0</v>
+      </c>
+      <c r="U148" s="15">
+        <v>3.7196929999999999</v>
+      </c>
+    </row>
+    <row r="149" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A149" s="13">
+        <v>5</v>
+      </c>
+      <c r="B149" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C149" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D149" s="15">
+        <v>1</v>
+      </c>
+      <c r="E149" s="15">
+        <v>6.6</v>
+      </c>
+      <c r="F149" s="15">
+        <v>8</v>
+      </c>
+      <c r="G149" s="15">
+        <v>0</v>
+      </c>
+      <c r="H149" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="I149" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J149" s="15">
+        <v>0</v>
+      </c>
+      <c r="K149" s="15">
+        <v>0</v>
+      </c>
+      <c r="L149" s="15">
+        <v>0</v>
+      </c>
+      <c r="M149" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N149" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="O149" s="15">
+        <v>0</v>
+      </c>
+      <c r="P149" s="15">
+        <v>2.9423319999999999</v>
+      </c>
+      <c r="Q149" s="15">
+        <v>0.36779149999999999</v>
+      </c>
+      <c r="R149" s="15">
+        <v>0</v>
+      </c>
+      <c r="S149" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="T149" s="15">
+        <v>0</v>
+      </c>
+      <c r="U149" s="15">
+        <v>3.9725760000000001</v>
+      </c>
+    </row>
+    <row r="150" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A150" s="13">
+        <v>6</v>
+      </c>
+      <c r="B150" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C150" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D150" s="15">
+        <v>1</v>
+      </c>
+      <c r="E150" s="15">
+        <v>7</v>
+      </c>
+      <c r="F150" s="15">
+        <v>8</v>
+      </c>
+      <c r="G150" s="15">
+        <v>0</v>
+      </c>
+      <c r="H150" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="I150" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J150" s="15">
+        <v>0</v>
+      </c>
+      <c r="K150" s="15">
+        <v>0</v>
+      </c>
+      <c r="L150" s="15">
+        <v>0</v>
+      </c>
+      <c r="M150" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N150" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="O150" s="15">
+        <v>0</v>
+      </c>
+      <c r="P150" s="15">
+        <v>2.9423319999999999</v>
+      </c>
+      <c r="Q150" s="15">
+        <v>0.36779149999999999</v>
+      </c>
+      <c r="R150" s="15">
+        <v>0</v>
+      </c>
+      <c r="S150" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="T150" s="15">
+        <v>0</v>
+      </c>
+      <c r="U150" s="15">
+        <v>4.2254589999999999</v>
+      </c>
+    </row>
+    <row r="151" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A151" s="13">
+        <v>7</v>
+      </c>
+      <c r="B151" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C151" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D151" s="15">
+        <v>1</v>
+      </c>
+      <c r="E151" s="15">
+        <v>7.4</v>
+      </c>
+      <c r="F151" s="15">
+        <v>8</v>
+      </c>
+      <c r="G151" s="15">
+        <v>0</v>
+      </c>
+      <c r="H151" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="I151" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J151" s="15">
+        <v>0</v>
+      </c>
+      <c r="K151" s="15">
+        <v>0</v>
+      </c>
+      <c r="L151" s="15">
+        <v>0</v>
+      </c>
+      <c r="M151" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N151" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="O151" s="15">
+        <v>0</v>
+      </c>
+      <c r="P151" s="15">
+        <v>2.9423319999999999</v>
+      </c>
+      <c r="Q151" s="15">
+        <v>0.36779149999999999</v>
+      </c>
+      <c r="R151" s="15">
+        <v>0</v>
+      </c>
+      <c r="S151" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="T151" s="15">
+        <v>0</v>
+      </c>
+      <c r="U151" s="15">
+        <v>4.4783429999999997</v>
+      </c>
+    </row>
+    <row r="152" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A152" s="13">
+        <v>8</v>
+      </c>
+      <c r="B152" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C152" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D152" s="15">
+        <v>1</v>
+      </c>
+      <c r="E152" s="15">
+        <v>7.8</v>
+      </c>
+      <c r="F152" s="15">
+        <v>8</v>
+      </c>
+      <c r="G152" s="15">
+        <v>0</v>
+      </c>
+      <c r="H152" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="I152" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J152" s="15">
+        <v>0</v>
+      </c>
+      <c r="K152" s="15">
+        <v>0</v>
+      </c>
+      <c r="L152" s="15">
+        <v>0</v>
+      </c>
+      <c r="M152" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N152" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="O152" s="15">
+        <v>0</v>
+      </c>
+      <c r="P152" s="15">
+        <v>2.9423319999999999</v>
+      </c>
+      <c r="Q152" s="15">
+        <v>0.36779149999999999</v>
+      </c>
+      <c r="R152" s="15">
+        <v>0</v>
+      </c>
+      <c r="S152" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="T152" s="15">
+        <v>0</v>
+      </c>
+      <c r="U152" s="15">
+        <v>4.7312260000000004</v>
+      </c>
+    </row>
+    <row r="153" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A153" s="13">
+        <v>9</v>
+      </c>
+      <c r="B153" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C153" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D153" s="15">
+        <v>1</v>
+      </c>
+      <c r="E153" s="15">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F153" s="15">
+        <v>8</v>
+      </c>
+      <c r="G153" s="15">
+        <v>0</v>
+      </c>
+      <c r="H153" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="I153" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J153" s="15">
+        <v>0</v>
+      </c>
+      <c r="K153" s="15">
+        <v>0</v>
+      </c>
+      <c r="L153" s="15">
+        <v>0</v>
+      </c>
+      <c r="M153" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N153" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="O153" s="15">
+        <v>0</v>
+      </c>
+      <c r="P153" s="15">
+        <v>2.9423319999999999</v>
+      </c>
+      <c r="Q153" s="15">
+        <v>0.36779149999999999</v>
+      </c>
+      <c r="R153" s="15">
+        <v>0</v>
+      </c>
+      <c r="S153" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="T153" s="15">
+        <v>0</v>
+      </c>
+      <c r="U153" s="15">
+        <v>4.9841100000000003</v>
+      </c>
+    </row>
+    <row r="154" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A154" s="13">
+        <v>10</v>
+      </c>
+      <c r="B154" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C154" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D154" s="15">
+        <v>1</v>
+      </c>
+      <c r="E154" s="15">
+        <v>8.6</v>
+      </c>
+      <c r="F154" s="15">
+        <v>8</v>
+      </c>
+      <c r="G154" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="H154" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="I154" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J154" s="15">
+        <v>0</v>
+      </c>
+      <c r="K154" s="15">
+        <v>0</v>
+      </c>
+      <c r="L154" s="15">
+        <v>0</v>
+      </c>
+      <c r="M154" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N154" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="O154" s="15">
+        <v>0</v>
+      </c>
+      <c r="P154" s="15">
+        <v>2.7502650000000002</v>
+      </c>
+      <c r="Q154" s="15">
+        <v>0.34378310000000001</v>
+      </c>
+      <c r="R154" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="S154" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="T154" s="15">
+        <v>0</v>
+      </c>
+      <c r="U154" s="15">
+        <v>5.2434649999999996</v>
+      </c>
+    </row>
+    <row r="155" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A155" s="13">
+        <v>11</v>
+      </c>
+      <c r="B155" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C155" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D155" s="15">
+        <v>1</v>
+      </c>
+      <c r="E155" s="15">
+        <v>9</v>
+      </c>
+      <c r="F155" s="15">
+        <v>8</v>
+      </c>
+      <c r="G155" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="H155" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="I155" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J155" s="15">
+        <v>0</v>
+      </c>
+      <c r="K155" s="15">
+        <v>0</v>
+      </c>
+      <c r="L155" s="15">
+        <v>0</v>
+      </c>
+      <c r="M155" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="N155" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="O155" s="15">
+        <v>0</v>
+      </c>
+      <c r="P155" s="15">
+        <v>2.7502650000000002</v>
+      </c>
+      <c r="Q155" s="15">
+        <v>0.34378310000000001</v>
+      </c>
+      <c r="R155" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="S155" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="T155" s="15">
+        <v>0</v>
+      </c>
+      <c r="U155" s="15">
+        <v>5.5059519999999997</v>
+      </c>
+    </row>
+    <row r="157" spans="1:21">
+      <c r="A157">
+        <v>1</v>
+      </c>
+      <c r="B157">
+        <v>-0.3</v>
+      </c>
+      <c r="C157">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D157">
+        <v>1</v>
+      </c>
+      <c r="E157">
+        <v>5</v>
+      </c>
+      <c r="F157">
+        <v>8</v>
+      </c>
+      <c r="G157">
+        <v>0</v>
+      </c>
+      <c r="H157">
+        <v>-0.5</v>
+      </c>
+      <c r="I157">
+        <v>0.5</v>
+      </c>
+      <c r="J157">
+        <v>0</v>
+      </c>
+      <c r="K157">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="L157">
+        <v>0</v>
+      </c>
+      <c r="M157">
+        <v>-0.2</v>
+      </c>
+      <c r="N157">
+        <v>0.371</v>
+      </c>
+      <c r="O157">
+        <v>0.8</v>
+      </c>
+      <c r="P157">
+        <v>4.8060299999999998</v>
+      </c>
+      <c r="Q157">
+        <v>0.60962870000000002</v>
+      </c>
+      <c r="R157">
+        <v>0</v>
+      </c>
+      <c r="S157">
+        <v>0</v>
+      </c>
+      <c r="T157">
+        <v>0</v>
+      </c>
+      <c r="U157">
+        <v>1.951856</v>
+      </c>
+    </row>
+    <row r="158" spans="1:21">
+      <c r="A158">
+        <v>2</v>
+      </c>
+      <c r="B158">
+        <v>-0.3</v>
+      </c>
+      <c r="C158">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D158">
+        <v>1</v>
+      </c>
+      <c r="E158">
+        <v>5.4</v>
+      </c>
+      <c r="F158">
+        <v>8</v>
+      </c>
+      <c r="G158">
+        <v>0</v>
+      </c>
+      <c r="H158">
+        <v>-0.5</v>
+      </c>
+      <c r="I158">
+        <v>0.5</v>
+      </c>
+      <c r="J158">
+        <v>0</v>
+      </c>
+      <c r="K158">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="L158">
+        <v>0</v>
+      </c>
+      <c r="M158">
+        <v>-0.2</v>
+      </c>
+      <c r="N158">
+        <v>0.371</v>
+      </c>
+      <c r="O158">
+        <v>0.8</v>
+      </c>
+      <c r="P158">
+        <v>4.8060299999999998</v>
+      </c>
+      <c r="Q158">
+        <v>0.60962870000000002</v>
+      </c>
+      <c r="R158">
+        <v>0</v>
+      </c>
+      <c r="S158">
+        <v>0</v>
+      </c>
+      <c r="T158">
+        <v>0</v>
+      </c>
+      <c r="U158">
+        <v>2.1080049999999999</v>
+      </c>
+    </row>
+    <row r="159" spans="1:21">
+      <c r="A159">
+        <v>3</v>
+      </c>
+      <c r="B159">
+        <v>-0.3</v>
+      </c>
+      <c r="C159">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
+      </c>
+      <c r="E159">
+        <v>5.8</v>
+      </c>
+      <c r="F159">
+        <v>8</v>
+      </c>
+      <c r="G159">
+        <v>0</v>
+      </c>
+      <c r="H159">
+        <v>-0.5</v>
+      </c>
+      <c r="I159">
+        <v>0.5</v>
+      </c>
+      <c r="J159">
+        <v>0</v>
+      </c>
+      <c r="K159">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="L159">
+        <v>0</v>
+      </c>
+      <c r="M159">
+        <v>-0.2</v>
+      </c>
+      <c r="N159">
+        <v>0.371</v>
+      </c>
+      <c r="O159">
+        <v>0.8</v>
+      </c>
+      <c r="P159">
+        <v>4.8060299999999998</v>
+      </c>
+      <c r="Q159">
+        <v>0.60962870000000002</v>
+      </c>
+      <c r="R159">
+        <v>0</v>
+      </c>
+      <c r="S159">
+        <v>0</v>
+      </c>
+      <c r="T159">
+        <v>0</v>
+      </c>
+      <c r="U159">
+        <v>2.2641529999999999</v>
+      </c>
+    </row>
+    <row r="160" spans="1:21">
+      <c r="A160">
+        <v>4</v>
+      </c>
+      <c r="B160">
+        <v>-0.3</v>
+      </c>
+      <c r="C160">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D160">
+        <v>1</v>
+      </c>
+      <c r="E160">
+        <v>6.2</v>
+      </c>
+      <c r="F160">
+        <v>8</v>
+      </c>
+      <c r="G160">
+        <v>0</v>
+      </c>
+      <c r="H160">
+        <v>-0.5</v>
+      </c>
+      <c r="I160">
+        <v>0.5</v>
+      </c>
+      <c r="J160">
+        <v>0</v>
+      </c>
+      <c r="K160">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="L160">
+        <v>0</v>
+      </c>
+      <c r="M160">
+        <v>-0.2</v>
+      </c>
+      <c r="N160">
+        <v>0.371</v>
+      </c>
+      <c r="O160">
+        <v>0.8</v>
+      </c>
+      <c r="P160">
+        <v>4.8060299999999998</v>
+      </c>
+      <c r="Q160">
+        <v>0.60962870000000002</v>
+      </c>
+      <c r="R160">
+        <v>0</v>
+      </c>
+      <c r="S160">
+        <v>0</v>
+      </c>
+      <c r="T160">
+        <v>0</v>
+      </c>
+      <c r="U160">
+        <v>2.420302</v>
+      </c>
+    </row>
+    <row r="161" spans="1:21">
+      <c r="A161">
+        <v>5</v>
+      </c>
+      <c r="B161">
+        <v>-0.3</v>
+      </c>
+      <c r="C161">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
+      <c r="E161">
+        <v>6.6</v>
+      </c>
+      <c r="F161">
+        <v>8</v>
+      </c>
+      <c r="G161">
+        <v>0</v>
+      </c>
+      <c r="H161">
+        <v>-0.5</v>
+      </c>
+      <c r="I161">
+        <v>0.5</v>
+      </c>
+      <c r="J161">
+        <v>0</v>
+      </c>
+      <c r="K161">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="L161">
+        <v>0</v>
+      </c>
+      <c r="M161">
+        <v>-0.2</v>
+      </c>
+      <c r="N161">
+        <v>0.371</v>
+      </c>
+      <c r="O161">
+        <v>0.8</v>
+      </c>
+      <c r="P161">
+        <v>4.8060299999999998</v>
+      </c>
+      <c r="Q161">
+        <v>0.60962870000000002</v>
+      </c>
+      <c r="R161">
+        <v>0</v>
+      </c>
+      <c r="S161">
+        <v>0</v>
+      </c>
+      <c r="T161">
+        <v>0</v>
+      </c>
+      <c r="U161">
+        <v>2.5764499999999999</v>
+      </c>
+    </row>
+    <row r="162" spans="1:21">
+      <c r="A162">
+        <v>6</v>
+      </c>
+      <c r="B162">
+        <v>-0.3</v>
+      </c>
+      <c r="C162">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D162">
+        <v>1</v>
+      </c>
+      <c r="E162">
+        <v>7</v>
+      </c>
+      <c r="F162">
+        <v>8</v>
+      </c>
+      <c r="G162">
+        <v>0</v>
+      </c>
+      <c r="H162">
+        <v>-0.5</v>
+      </c>
+      <c r="I162">
+        <v>0.5</v>
+      </c>
+      <c r="J162">
+        <v>0</v>
+      </c>
+      <c r="K162">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="L162">
+        <v>0</v>
+      </c>
+      <c r="M162">
+        <v>-0.2</v>
+      </c>
+      <c r="N162">
+        <v>0.371</v>
+      </c>
+      <c r="O162">
+        <v>0.8</v>
+      </c>
+      <c r="P162">
+        <v>4.8060299999999998</v>
+      </c>
+      <c r="Q162">
+        <v>0.60962870000000002</v>
+      </c>
+      <c r="R162">
+        <v>0</v>
+      </c>
+      <c r="S162">
+        <v>0</v>
+      </c>
+      <c r="T162">
+        <v>0</v>
+      </c>
+      <c r="U162">
+        <v>2.732599</v>
+      </c>
+    </row>
+    <row r="163" spans="1:21">
+      <c r="A163">
+        <v>7</v>
+      </c>
+      <c r="B163">
+        <v>-0.3</v>
+      </c>
+      <c r="C163">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D163">
+        <v>1</v>
+      </c>
+      <c r="E163">
+        <v>7.4</v>
+      </c>
+      <c r="F163">
+        <v>8</v>
+      </c>
+      <c r="G163">
+        <v>0</v>
+      </c>
+      <c r="H163">
+        <v>-0.5</v>
+      </c>
+      <c r="I163">
+        <v>0.5</v>
+      </c>
+      <c r="J163">
+        <v>0</v>
+      </c>
+      <c r="K163">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="L163">
+        <v>0</v>
+      </c>
+      <c r="M163">
+        <v>-0.2</v>
+      </c>
+      <c r="N163">
+        <v>0.371</v>
+      </c>
+      <c r="O163">
+        <v>0.8</v>
+      </c>
+      <c r="P163">
+        <v>4.8060299999999998</v>
+      </c>
+      <c r="Q163">
+        <v>0.60962870000000002</v>
+      </c>
+      <c r="R163">
+        <v>0</v>
+      </c>
+      <c r="S163">
+        <v>0</v>
+      </c>
+      <c r="T163">
+        <v>0</v>
+      </c>
+      <c r="U163">
+        <v>2.888747</v>
+      </c>
+    </row>
+    <row r="164" spans="1:21">
+      <c r="A164">
+        <v>8</v>
+      </c>
+      <c r="B164">
+        <v>-0.3</v>
+      </c>
+      <c r="C164">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D164">
+        <v>1</v>
+      </c>
+      <c r="E164">
+        <v>7.8</v>
+      </c>
+      <c r="F164">
+        <v>8</v>
+      </c>
+      <c r="G164">
+        <v>0</v>
+      </c>
+      <c r="H164">
+        <v>-0.3</v>
+      </c>
+      <c r="I164">
+        <v>0.5</v>
+      </c>
+      <c r="J164">
+        <v>0</v>
+      </c>
+      <c r="K164">
+        <v>2.4E-2</v>
+      </c>
+      <c r="L164">
+        <v>0</v>
+      </c>
+      <c r="M164">
+        <v>-0.2</v>
+      </c>
+      <c r="N164">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="O164">
+        <v>0.6</v>
+      </c>
+      <c r="P164">
+        <v>4.6387010000000002</v>
+      </c>
+      <c r="Q164">
+        <v>0.58283759999999996</v>
+      </c>
+      <c r="R164">
+        <v>0</v>
+      </c>
+      <c r="S164">
+        <v>0.2</v>
+      </c>
+      <c r="T164">
+        <v>0</v>
+      </c>
+      <c r="U164">
+        <v>3.0538660000000002</v>
+      </c>
+    </row>
+    <row r="165" spans="1:21">
+      <c r="A165">
+        <v>9</v>
+      </c>
+      <c r="B165">
+        <v>-0.3</v>
+      </c>
+      <c r="C165">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D165">
+        <v>1</v>
+      </c>
+      <c r="E165">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F165">
+        <v>8</v>
+      </c>
+      <c r="G165">
+        <v>0</v>
+      </c>
+      <c r="H165">
+        <v>-0.1</v>
+      </c>
+      <c r="I165">
+        <v>0.5</v>
+      </c>
+      <c r="J165">
+        <v>0</v>
+      </c>
+      <c r="K165">
+        <v>0</v>
+      </c>
+      <c r="L165">
+        <v>0</v>
+      </c>
+      <c r="M165">
+        <v>-0.2</v>
+      </c>
+      <c r="N165">
+        <v>0.3</v>
+      </c>
+      <c r="O165">
+        <v>0.4</v>
+      </c>
+      <c r="P165">
+        <v>4.4634530000000003</v>
+      </c>
+      <c r="Q165">
+        <v>0.55793159999999997</v>
+      </c>
+      <c r="R165">
+        <v>0</v>
+      </c>
+      <c r="S165">
+        <v>0.4</v>
+      </c>
+      <c r="T165">
+        <v>0</v>
+      </c>
+      <c r="U165">
+        <v>3.224961</v>
+      </c>
+    </row>
+    <row r="166" spans="1:21">
+      <c r="A166">
+        <v>10</v>
+      </c>
+      <c r="B166">
+        <v>-0.3</v>
+      </c>
+      <c r="C166">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D166">
+        <v>1</v>
+      </c>
+      <c r="E166">
+        <v>8.6</v>
+      </c>
+      <c r="F166">
+        <v>8</v>
+      </c>
+      <c r="G166">
+        <v>0.8</v>
+      </c>
+      <c r="H166">
+        <v>0.3</v>
+      </c>
+      <c r="I166">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J166">
+        <v>0</v>
+      </c>
+      <c r="K166">
+        <v>0</v>
+      </c>
+      <c r="L166">
+        <v>0</v>
+      </c>
+      <c r="M166">
+        <v>-0.8</v>
+      </c>
+      <c r="N166">
+        <v>-0.5</v>
+      </c>
+      <c r="O166">
+        <v>0</v>
+      </c>
+      <c r="P166">
+        <v>2.7502650000000002</v>
+      </c>
+      <c r="Q166">
+        <v>0.34378310000000001</v>
+      </c>
+      <c r="R166">
+        <v>0.8</v>
+      </c>
+      <c r="S166">
+        <v>0.8</v>
+      </c>
+      <c r="T166">
+        <v>0.6</v>
+      </c>
+      <c r="U166">
+        <v>3.4434650000000002</v>
+      </c>
+    </row>
+    <row r="167" spans="1:21">
+      <c r="A167">
+        <v>11</v>
+      </c>
+      <c r="B167">
+        <v>-0.3</v>
+      </c>
+      <c r="C167">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D167">
+        <v>1</v>
+      </c>
+      <c r="E167">
+        <v>9</v>
+      </c>
+      <c r="F167">
+        <v>8</v>
+      </c>
+      <c r="G167">
+        <v>0.8</v>
+      </c>
+      <c r="H167">
+        <v>0.3</v>
+      </c>
+      <c r="I167">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J167">
+        <v>0</v>
+      </c>
+      <c r="K167">
+        <v>0</v>
+      </c>
+      <c r="L167">
+        <v>0</v>
+      </c>
+      <c r="M167">
+        <v>-0.8</v>
+      </c>
+      <c r="N167">
+        <v>-0.5</v>
+      </c>
+      <c r="O167">
+        <v>0</v>
+      </c>
+      <c r="P167">
+        <v>2.7502650000000002</v>
+      </c>
+      <c r="Q167">
+        <v>0.34378310000000001</v>
+      </c>
+      <c r="R167">
+        <v>0.8</v>
+      </c>
+      <c r="S167">
+        <v>0.8</v>
+      </c>
+      <c r="T167">
+        <v>0.6</v>
+      </c>
+      <c r="U167">
+        <v>3.7059519999999999</v>
+      </c>
+    </row>
+    <row r="168" spans="1:21" ht="15.75" thickBot="1"/>
+    <row r="169" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A169" s="13">
+        <v>1</v>
+      </c>
+      <c r="B169" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="C169" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D169" s="15">
+        <v>1</v>
+      </c>
+      <c r="E169" s="15">
+        <v>5</v>
+      </c>
+      <c r="F169" s="15">
+        <v>9</v>
+      </c>
+      <c r="G169" s="15">
+        <v>0</v>
+      </c>
+      <c r="H169" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I169" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J169" s="15">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="K169" s="15">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="L169" s="15">
+        <v>0</v>
+      </c>
+      <c r="M169" s="15">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="N169" s="15">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="O169" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="P169" s="15">
+        <v>5.4417010000000001</v>
+      </c>
+      <c r="Q169" s="15">
+        <v>0.6864112</v>
+      </c>
+      <c r="R169" s="15">
+        <v>0</v>
+      </c>
+      <c r="S169" s="15">
+        <v>0</v>
+      </c>
+      <c r="T169" s="15">
+        <v>0</v>
+      </c>
+      <c r="U169" s="15">
+        <v>1.567944</v>
+      </c>
+    </row>
+    <row r="170" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A170" s="13">
+        <v>2</v>
+      </c>
+      <c r="B170" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="C170" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D170" s="15">
+        <v>1</v>
+      </c>
+      <c r="E170" s="15">
+        <v>5.4</v>
+      </c>
+      <c r="F170" s="15">
+        <v>9</v>
+      </c>
+      <c r="G170" s="15">
+        <v>0</v>
+      </c>
+      <c r="H170" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I170" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="J170" s="15">
+        <v>0</v>
+      </c>
+      <c r="K170" s="15">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="L170" s="15">
+        <v>0</v>
+      </c>
+      <c r="M170" s="15">
+        <v>-0.4</v>
+      </c>
+      <c r="N170" s="15">
+        <v>0.872</v>
+      </c>
+      <c r="O170" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="P170" s="15">
+        <v>5.2545510000000002</v>
+      </c>
+      <c r="Q170" s="15">
+        <v>0.64739460000000004</v>
+      </c>
+      <c r="R170" s="15">
+        <v>0</v>
+      </c>
+      <c r="S170" s="15">
+        <v>0</v>
+      </c>
+      <c r="T170" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="U170" s="15">
+        <v>1.7040690000000001</v>
+      </c>
+    </row>
+    <row r="171" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A171" s="13">
+        <v>3</v>
+      </c>
+      <c r="B171" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="C171" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D171" s="15">
+        <v>1</v>
+      </c>
+      <c r="E171" s="15">
+        <v>5.8</v>
+      </c>
+      <c r="F171" s="15">
+        <v>9</v>
+      </c>
+      <c r="G171" s="15">
+        <v>0</v>
+      </c>
+      <c r="H171" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I171" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="J171" s="15">
+        <v>0</v>
+      </c>
+      <c r="K171" s="15">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="L171" s="15">
+        <v>0</v>
+      </c>
+      <c r="M171" s="15">
+        <v>-0.4</v>
+      </c>
+      <c r="N171" s="15">
+        <v>0.872</v>
+      </c>
+      <c r="O171" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="P171" s="15">
+        <v>5.2545510000000002</v>
+      </c>
+      <c r="Q171" s="15">
+        <v>0.64739460000000004</v>
+      </c>
+      <c r="R171" s="15">
+        <v>0</v>
+      </c>
+      <c r="S171" s="15">
+        <v>0</v>
+      </c>
+      <c r="T171" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="U171" s="15">
+        <v>1.8451120000000001</v>
+      </c>
+    </row>
+    <row r="172" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A172" s="13">
+        <v>4</v>
+      </c>
+      <c r="B172" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="C172" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D172" s="15">
+        <v>1</v>
+      </c>
+      <c r="E172" s="15">
+        <v>6.2</v>
+      </c>
+      <c r="F172" s="15">
+        <v>9</v>
+      </c>
+      <c r="G172" s="15">
+        <v>0</v>
+      </c>
+      <c r="H172" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I172" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="J172" s="15">
+        <v>0</v>
+      </c>
+      <c r="K172" s="15">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="L172" s="15">
+        <v>0</v>
+      </c>
+      <c r="M172" s="15">
+        <v>-0.4</v>
+      </c>
+      <c r="N172" s="15">
+        <v>0.872</v>
+      </c>
+      <c r="O172" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="P172" s="15">
+        <v>5.2545510000000002</v>
+      </c>
+      <c r="Q172" s="15">
+        <v>0.64739460000000004</v>
+      </c>
+      <c r="R172" s="15">
+        <v>0</v>
+      </c>
+      <c r="S172" s="15">
+        <v>0</v>
+      </c>
+      <c r="T172" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="U172" s="15">
+        <v>1.986154</v>
+      </c>
+    </row>
+    <row r="173" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A173" s="13">
+        <v>5</v>
+      </c>
+      <c r="B173" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="C173" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D173" s="15">
+        <v>1</v>
+      </c>
+      <c r="E173" s="15">
+        <v>6.6</v>
+      </c>
+      <c r="F173" s="15">
+        <v>9</v>
+      </c>
+      <c r="G173" s="15">
+        <v>0</v>
+      </c>
+      <c r="H173" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I173" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="J173" s="15">
+        <v>0</v>
+      </c>
+      <c r="K173" s="15">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="L173" s="15">
+        <v>0</v>
+      </c>
+      <c r="M173" s="15">
+        <v>-0.4</v>
+      </c>
+      <c r="N173" s="15">
+        <v>0.872</v>
+      </c>
+      <c r="O173" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="P173" s="15">
+        <v>5.2545510000000002</v>
+      </c>
+      <c r="Q173" s="15">
+        <v>0.64739460000000004</v>
+      </c>
+      <c r="R173" s="15">
+        <v>0</v>
+      </c>
+      <c r="S173" s="15">
+        <v>0</v>
+      </c>
+      <c r="T173" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="U173" s="15">
+        <v>2.1271960000000001</v>
+      </c>
+    </row>
+    <row r="174" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A174" s="13">
+        <v>6</v>
+      </c>
+      <c r="B174" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="C174" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D174" s="15">
+        <v>1</v>
+      </c>
+      <c r="E174" s="15">
+        <v>7</v>
+      </c>
+      <c r="F174" s="15">
+        <v>9</v>
+      </c>
+      <c r="G174" s="15">
+        <v>0</v>
+      </c>
+      <c r="H174" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I174" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="J174" s="15">
+        <v>0</v>
+      </c>
+      <c r="K174" s="15">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="L174" s="15">
+        <v>0</v>
+      </c>
+      <c r="M174" s="15">
+        <v>-0.4</v>
+      </c>
+      <c r="N174" s="15">
+        <v>0.872</v>
+      </c>
+      <c r="O174" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="P174" s="15">
+        <v>5.2545510000000002</v>
+      </c>
+      <c r="Q174" s="15">
+        <v>0.64739460000000004</v>
+      </c>
+      <c r="R174" s="15">
+        <v>0</v>
+      </c>
+      <c r="S174" s="15">
+        <v>0</v>
+      </c>
+      <c r="T174" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="U174" s="15">
+        <v>2.2682380000000002</v>
+      </c>
+    </row>
+    <row r="175" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A175" s="13">
+        <v>7</v>
+      </c>
+      <c r="B175" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="C175" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D175" s="15">
+        <v>1</v>
+      </c>
+      <c r="E175" s="15">
+        <v>7.4</v>
+      </c>
+      <c r="F175" s="15">
+        <v>9</v>
+      </c>
+      <c r="G175" s="15">
+        <v>0</v>
+      </c>
+      <c r="H175" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I175" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="J175" s="15">
+        <v>0</v>
+      </c>
+      <c r="K175" s="15">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="L175" s="15">
+        <v>0</v>
+      </c>
+      <c r="M175" s="15">
+        <v>-0.4</v>
+      </c>
+      <c r="N175" s="15">
+        <v>0.872</v>
+      </c>
+      <c r="O175" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="P175" s="15">
+        <v>5.2545510000000002</v>
+      </c>
+      <c r="Q175" s="15">
+        <v>0.64739460000000004</v>
+      </c>
+      <c r="R175" s="15">
+        <v>0</v>
+      </c>
+      <c r="S175" s="15">
+        <v>0</v>
+      </c>
+      <c r="T175" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="U175" s="15">
+        <v>2.4092799999999999</v>
+      </c>
+    </row>
+    <row r="176" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A176" s="13">
+        <v>8</v>
+      </c>
+      <c r="B176" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="C176" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D176" s="15">
+        <v>1</v>
+      </c>
+      <c r="E176" s="15">
+        <v>7.8</v>
+      </c>
+      <c r="F176" s="15">
+        <v>9</v>
+      </c>
+      <c r="G176" s="15">
+        <v>0</v>
+      </c>
+      <c r="H176" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I176" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="J176" s="15">
+        <v>0</v>
+      </c>
+      <c r="K176" s="15">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="L176" s="15">
+        <v>0</v>
+      </c>
+      <c r="M176" s="15">
+        <v>-0.4</v>
+      </c>
+      <c r="N176" s="15">
+        <v>0.872</v>
+      </c>
+      <c r="O176" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="P176" s="15">
+        <v>5.2545510000000002</v>
+      </c>
+      <c r="Q176" s="15">
+        <v>0.64739460000000004</v>
+      </c>
+      <c r="R176" s="15">
+        <v>0</v>
+      </c>
+      <c r="S176" s="15">
+        <v>0</v>
+      </c>
+      <c r="T176" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="U176" s="15">
+        <v>2.550322</v>
+      </c>
+    </row>
+    <row r="177" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A177" s="13">
+        <v>9</v>
+      </c>
+      <c r="B177" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="C177" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D177" s="15">
+        <v>1</v>
+      </c>
+      <c r="E177" s="15">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F177" s="15">
+        <v>9</v>
+      </c>
+      <c r="G177" s="15">
+        <v>0</v>
+      </c>
+      <c r="H177" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I177" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="J177" s="15">
+        <v>0</v>
+      </c>
+      <c r="K177" s="15">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="L177" s="15">
+        <v>0</v>
+      </c>
+      <c r="M177" s="15">
+        <v>-0.4</v>
+      </c>
+      <c r="N177" s="15">
+        <v>0.872</v>
+      </c>
+      <c r="O177" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="P177" s="15">
+        <v>5.2545510000000002</v>
+      </c>
+      <c r="Q177" s="15">
+        <v>0.64739460000000004</v>
+      </c>
+      <c r="R177" s="15">
+        <v>0</v>
+      </c>
+      <c r="S177" s="15">
+        <v>0</v>
+      </c>
+      <c r="T177" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="U177" s="15">
+        <v>2.6913649999999998</v>
+      </c>
+    </row>
+    <row r="178" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A178" s="13">
+        <v>10</v>
+      </c>
+      <c r="B178" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="C178" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D178" s="15">
+        <v>1</v>
+      </c>
+      <c r="E178" s="15">
+        <v>8.6</v>
+      </c>
+      <c r="F178" s="15">
+        <v>9</v>
+      </c>
+      <c r="G178" s="15">
+        <v>0</v>
+      </c>
+      <c r="H178" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I178" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="J178" s="15">
+        <v>0</v>
+      </c>
+      <c r="K178" s="15">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="L178" s="15">
+        <v>0</v>
+      </c>
+      <c r="M178" s="15">
+        <v>-0.4</v>
+      </c>
+      <c r="N178" s="15">
+        <v>0.872</v>
+      </c>
+      <c r="O178" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="P178" s="15">
+        <v>5.2545510000000002</v>
+      </c>
+      <c r="Q178" s="15">
+        <v>0.64739460000000004</v>
+      </c>
+      <c r="R178" s="15">
+        <v>0</v>
+      </c>
+      <c r="S178" s="15">
+        <v>0</v>
+      </c>
+      <c r="T178" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="U178" s="15">
+        <v>2.8324069999999999</v>
+      </c>
+    </row>
+    <row r="179" spans="1:21" ht="15.75" thickBot="1">
+      <c r="A179" s="13">
+        <v>11</v>
+      </c>
+      <c r="B179" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="C179" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D179" s="15">
+        <v>1</v>
+      </c>
+      <c r="E179" s="15">
+        <v>9</v>
+      </c>
+      <c r="F179" s="15">
+        <v>9</v>
+      </c>
+      <c r="G179" s="15">
+        <v>0</v>
+      </c>
+      <c r="H179" s="15">
+        <v>-0.5</v>
+      </c>
+      <c r="I179" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="J179" s="15">
+        <v>0</v>
+      </c>
+      <c r="K179" s="15">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="L179" s="15">
+        <v>0</v>
+      </c>
+      <c r="M179" s="15">
+        <v>-0.4</v>
+      </c>
+      <c r="N179" s="15">
+        <v>0.872</v>
+      </c>
+      <c r="O179" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="P179" s="15">
+        <v>5.2545510000000002</v>
+      </c>
+      <c r="Q179" s="15">
+        <v>0.64739460000000004</v>
+      </c>
+      <c r="R179" s="15">
+        <v>0</v>
+      </c>
+      <c r="S179" s="15">
+        <v>0</v>
+      </c>
+      <c r="T179" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="U179" s="15">
+        <v>2.973449</v>
+      </c>
+    </row>
+    <row r="181" spans="1:21">
+      <c r="A181">
+        <v>1</v>
+      </c>
+      <c r="B181">
+        <v>-0.3</v>
+      </c>
+      <c r="C181">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D181">
+        <v>0.9</v>
+      </c>
+      <c r="E181">
+        <v>5</v>
+      </c>
+      <c r="F181">
+        <v>9</v>
+      </c>
+      <c r="G181">
+        <v>0</v>
+      </c>
+      <c r="H181">
+        <v>-0.5</v>
+      </c>
+      <c r="I181">
+        <v>0.5</v>
+      </c>
+      <c r="J181">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="K181">
+        <v>0</v>
+      </c>
+      <c r="L181">
+        <v>0</v>
+      </c>
+      <c r="M181">
+        <v>0.752</v>
+      </c>
+      <c r="N181">
+        <v>0.3</v>
+      </c>
+      <c r="O181">
+        <v>0.8</v>
+      </c>
+      <c r="P181">
+        <v>5.5096889999999998</v>
+      </c>
+      <c r="Q181">
+        <v>0.71796543999999995</v>
+      </c>
+      <c r="R181">
+        <v>0</v>
+      </c>
+      <c r="S181">
+        <v>0</v>
+      </c>
+      <c r="T181">
+        <v>0</v>
+      </c>
+      <c r="U181">
+        <v>1.4101729999999999</v>
+      </c>
+    </row>
+    <row r="182" spans="1:21">
+      <c r="A182">
+        <v>2</v>
+      </c>
+      <c r="B182">
+        <v>-0.3</v>
+      </c>
+      <c r="C182">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D182">
+        <v>0.9</v>
+      </c>
+      <c r="E182">
+        <v>5.4</v>
+      </c>
+      <c r="F182">
+        <v>9</v>
+      </c>
+      <c r="G182">
+        <v>0</v>
+      </c>
+      <c r="H182">
+        <v>-0.5</v>
+      </c>
+      <c r="I182">
+        <v>0.5</v>
+      </c>
+      <c r="J182">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="K182">
+        <v>0</v>
+      </c>
+      <c r="L182">
+        <v>0</v>
+      </c>
+      <c r="M182">
+        <v>0.752</v>
+      </c>
+      <c r="N182">
+        <v>0.3</v>
+      </c>
+      <c r="O182">
+        <v>0.8</v>
+      </c>
+      <c r="P182">
+        <v>5.5096889999999998</v>
+      </c>
+      <c r="Q182">
+        <v>0.71796543999999995</v>
+      </c>
+      <c r="R182">
+        <v>0</v>
+      </c>
+      <c r="S182">
+        <v>0</v>
+      </c>
+      <c r="T182">
+        <v>0</v>
+      </c>
+      <c r="U182">
+        <v>1.5229870000000001</v>
+      </c>
+    </row>
+    <row r="183" spans="1:21">
+      <c r="A183">
+        <v>3</v>
+      </c>
+      <c r="B183">
+        <v>-0.3</v>
+      </c>
+      <c r="C183">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D183">
+        <v>0.9</v>
+      </c>
+      <c r="E183">
+        <v>5.8</v>
+      </c>
+      <c r="F183">
+        <v>9</v>
+      </c>
+      <c r="G183">
+        <v>0</v>
+      </c>
+      <c r="H183">
+        <v>-0.5</v>
+      </c>
+      <c r="I183">
+        <v>0.5</v>
+      </c>
+      <c r="J183">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="K183">
+        <v>0</v>
+      </c>
+      <c r="L183">
+        <v>0</v>
+      </c>
+      <c r="M183">
+        <v>0.752</v>
+      </c>
+      <c r="N183">
+        <v>0.3</v>
+      </c>
+      <c r="O183">
+        <v>0.8</v>
+      </c>
+      <c r="P183">
+        <v>5.5096889999999998</v>
+      </c>
+      <c r="Q183">
+        <v>0.71796543999999995</v>
+      </c>
+      <c r="R183">
+        <v>0</v>
+      </c>
+      <c r="S183">
+        <v>0</v>
+      </c>
+      <c r="T183">
+        <v>0</v>
+      </c>
+      <c r="U183">
+        <v>1.6357999999999999</v>
+      </c>
+    </row>
+    <row r="184" spans="1:21">
+      <c r="A184">
+        <v>4</v>
+      </c>
+      <c r="B184">
+        <v>-0.3</v>
+      </c>
+      <c r="C184">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D184">
+        <v>0.9</v>
+      </c>
+      <c r="E184">
+        <v>6.2</v>
+      </c>
+      <c r="F184">
+        <v>9</v>
+      </c>
+      <c r="G184">
+        <v>0</v>
+      </c>
+      <c r="H184">
+        <v>-0.5</v>
+      </c>
+      <c r="I184">
+        <v>0.5</v>
+      </c>
+      <c r="J184">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="K184">
+        <v>0</v>
+      </c>
+      <c r="L184">
+        <v>0</v>
+      </c>
+      <c r="M184">
+        <v>0.752</v>
+      </c>
+      <c r="N184">
+        <v>0.3</v>
+      </c>
+      <c r="O184">
+        <v>0.8</v>
+      </c>
+      <c r="P184">
+        <v>5.5096889999999998</v>
+      </c>
+      <c r="Q184">
+        <v>0.71796543999999995</v>
+      </c>
+      <c r="R184">
+        <v>0</v>
+      </c>
+      <c r="S184">
+        <v>0</v>
+      </c>
+      <c r="T184">
+        <v>0</v>
+      </c>
+      <c r="U184">
+        <v>1.7486139999999999</v>
+      </c>
+    </row>
+    <row r="185" spans="1:21">
+      <c r="A185">
+        <v>5</v>
+      </c>
+      <c r="B185">
+        <v>-0.3</v>
+      </c>
+      <c r="C185">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D185">
+        <v>0.9</v>
+      </c>
+      <c r="E185">
+        <v>6.6</v>
+      </c>
+      <c r="F185">
+        <v>9</v>
+      </c>
+      <c r="G185">
+        <v>0</v>
+      </c>
+      <c r="H185">
+        <v>-0.5</v>
+      </c>
+      <c r="I185">
+        <v>0.5</v>
+      </c>
+      <c r="J185">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="K185">
+        <v>0</v>
+      </c>
+      <c r="L185">
+        <v>0</v>
+      </c>
+      <c r="M185">
+        <v>0.752</v>
+      </c>
+      <c r="N185">
+        <v>0.3</v>
+      </c>
+      <c r="O185">
+        <v>0.8</v>
+      </c>
+      <c r="P185">
+        <v>5.5096889999999998</v>
+      </c>
+      <c r="Q185">
+        <v>0.71796543999999995</v>
+      </c>
+      <c r="R185">
+        <v>0</v>
+      </c>
+      <c r="S185">
+        <v>0</v>
+      </c>
+      <c r="T185">
+        <v>0</v>
+      </c>
+      <c r="U185">
+        <v>1.8614280000000001</v>
+      </c>
+    </row>
+    <row r="186" spans="1:21">
+      <c r="A186">
+        <v>6</v>
+      </c>
+      <c r="B186">
+        <v>-0.3</v>
+      </c>
+      <c r="C186">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D186">
+        <v>0.9</v>
+      </c>
+      <c r="E186">
+        <v>7</v>
+      </c>
+      <c r="F186">
+        <v>9</v>
+      </c>
+      <c r="G186">
+        <v>0</v>
+      </c>
+      <c r="H186">
+        <v>-0.5</v>
+      </c>
+      <c r="I186">
+        <v>0.5</v>
+      </c>
+      <c r="J186">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="K186">
+        <v>0</v>
+      </c>
+      <c r="L186">
+        <v>0</v>
+      </c>
+      <c r="M186">
+        <v>0.752</v>
+      </c>
+      <c r="N186">
+        <v>0.3</v>
+      </c>
+      <c r="O186">
+        <v>0.8</v>
+      </c>
+      <c r="P186">
+        <v>5.5096889999999998</v>
+      </c>
+      <c r="Q186">
+        <v>0.71796543999999995</v>
+      </c>
+      <c r="R186">
+        <v>0</v>
+      </c>
+      <c r="S186">
+        <v>0</v>
+      </c>
+      <c r="T186">
+        <v>0</v>
+      </c>
+      <c r="U186">
+        <v>1.9742420000000001</v>
+      </c>
+    </row>
+    <row r="187" spans="1:21">
+      <c r="A187">
+        <v>7</v>
+      </c>
+      <c r="B187">
+        <v>-0.3</v>
+      </c>
+      <c r="C187">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D187">
+        <v>0.9</v>
+      </c>
+      <c r="E187">
+        <v>7.4</v>
+      </c>
+      <c r="F187">
+        <v>9</v>
+      </c>
+      <c r="G187">
+        <v>0</v>
+      </c>
+      <c r="H187">
+        <v>-0.5</v>
+      </c>
+      <c r="I187">
+        <v>0.5</v>
+      </c>
+      <c r="J187">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="K187">
+        <v>0</v>
+      </c>
+      <c r="L187">
+        <v>0</v>
+      </c>
+      <c r="M187">
+        <v>0.752</v>
+      </c>
+      <c r="N187">
+        <v>0.3</v>
+      </c>
+      <c r="O187">
+        <v>0.8</v>
+      </c>
+      <c r="P187">
+        <v>5.5096889999999998</v>
+      </c>
+      <c r="Q187">
+        <v>0.71796543999999995</v>
+      </c>
+      <c r="R187">
+        <v>0</v>
+      </c>
+      <c r="S187">
+        <v>0</v>
+      </c>
+      <c r="T187">
+        <v>0</v>
+      </c>
+      <c r="U187">
+        <v>2.087056</v>
+      </c>
+    </row>
+    <row r="188" spans="1:21">
+      <c r="A188">
+        <v>8</v>
+      </c>
+      <c r="B188">
+        <v>-0.3</v>
+      </c>
+      <c r="C188">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D188">
+        <v>0.9</v>
+      </c>
+      <c r="E188">
+        <v>7.8</v>
+      </c>
+      <c r="F188">
+        <v>9</v>
+      </c>
+      <c r="G188">
+        <v>0</v>
+      </c>
+      <c r="H188">
+        <v>-0.5</v>
+      </c>
+      <c r="I188">
+        <v>0.5</v>
+      </c>
+      <c r="J188">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="K188">
+        <v>0</v>
+      </c>
+      <c r="L188">
+        <v>0</v>
+      </c>
+      <c r="M188">
+        <v>0.752</v>
+      </c>
+      <c r="N188">
+        <v>0.3</v>
+      </c>
+      <c r="O188">
+        <v>0.8</v>
+      </c>
+      <c r="P188">
+        <v>5.5096889999999998</v>
+      </c>
+      <c r="Q188">
+        <v>0.71796543999999995</v>
+      </c>
+      <c r="R188">
+        <v>0</v>
+      </c>
+      <c r="S188">
+        <v>0</v>
+      </c>
+      <c r="T188">
+        <v>0</v>
+      </c>
+      <c r="U188">
+        <v>2.1998700000000002</v>
+      </c>
+    </row>
+    <row r="189" spans="1:21">
+      <c r="A189">
+        <v>9</v>
+      </c>
+      <c r="B189">
+        <v>-0.3</v>
+      </c>
+      <c r="C189">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D189">
+        <v>0.9</v>
+      </c>
+      <c r="E189">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F189">
+        <v>9</v>
+      </c>
+      <c r="G189">
+        <v>0</v>
+      </c>
+      <c r="H189">
+        <v>-0.5</v>
+      </c>
+      <c r="I189">
+        <v>0.5</v>
+      </c>
+      <c r="J189">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="K189">
+        <v>0</v>
+      </c>
+      <c r="L189">
+        <v>0</v>
+      </c>
+      <c r="M189">
+        <v>0.752</v>
+      </c>
+      <c r="N189">
+        <v>0.3</v>
+      </c>
+      <c r="O189">
+        <v>0.8</v>
+      </c>
+      <c r="P189">
+        <v>5.5096889999999998</v>
+      </c>
+      <c r="Q189">
+        <v>0.71796543999999995</v>
+      </c>
+      <c r="R189">
+        <v>0</v>
+      </c>
+      <c r="S189">
+        <v>0</v>
+      </c>
+      <c r="T189">
+        <v>0</v>
+      </c>
+      <c r="U189">
+        <v>2.3126829999999998</v>
+      </c>
+    </row>
+    <row r="190" spans="1:21">
+      <c r="A190">
+        <v>10</v>
+      </c>
+      <c r="B190">
+        <v>-0.3</v>
+      </c>
+      <c r="C190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D190">
+        <v>0.9</v>
+      </c>
+      <c r="E190">
+        <v>8.6</v>
+      </c>
+      <c r="F190">
+        <v>9</v>
+      </c>
+      <c r="G190">
+        <v>2</v>
+      </c>
+      <c r="H190">
+        <v>1.5</v>
+      </c>
+      <c r="I190">
+        <v>1.9</v>
+      </c>
+      <c r="J190">
+        <v>0</v>
+      </c>
+      <c r="K190">
+        <v>0</v>
+      </c>
+      <c r="L190">
+        <v>0</v>
+      </c>
+      <c r="M190">
+        <v>-1.6</v>
+      </c>
+      <c r="N190">
+        <v>-1.7</v>
+      </c>
+      <c r="O190">
+        <v>-1.2</v>
+      </c>
+      <c r="P190">
+        <v>0.77665490000000004</v>
+      </c>
+      <c r="Q190">
+        <v>8.6294990000000002E-2</v>
+      </c>
+      <c r="R190">
+        <v>2</v>
+      </c>
+      <c r="S190">
+        <v>2</v>
+      </c>
+      <c r="T190">
+        <v>1.4</v>
+      </c>
+      <c r="U190">
+        <v>2.4578630000000001</v>
+      </c>
+    </row>
+    <row r="191" spans="1:21">
+      <c r="A191">
+        <v>11</v>
+      </c>
+      <c r="B191">
+        <v>-0.3</v>
+      </c>
+      <c r="C191">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D191">
+        <v>0.9</v>
+      </c>
+      <c r="E191">
+        <v>9</v>
+      </c>
+      <c r="F191">
+        <v>9</v>
+      </c>
+      <c r="G191">
+        <v>2</v>
+      </c>
+      <c r="H191">
+        <v>1.5</v>
+      </c>
+      <c r="I191">
+        <v>1.9</v>
+      </c>
+      <c r="J191">
+        <v>0</v>
+      </c>
+      <c r="K191">
+        <v>0</v>
+      </c>
+      <c r="L191">
+        <v>0</v>
+      </c>
+      <c r="M191">
+        <v>-1.6</v>
+      </c>
+      <c r="N191">
+        <v>-1.7</v>
+      </c>
+      <c r="O191">
+        <v>-1.2</v>
+      </c>
+      <c r="P191">
+        <v>0.77665490000000004</v>
+      </c>
+      <c r="Q191">
+        <v>8.6294990000000002E-2</v>
+      </c>
+      <c r="R191">
+        <v>2</v>
+      </c>
+      <c r="S191">
+        <v>2</v>
+      </c>
+      <c r="T191">
+        <v>1.4</v>
+      </c>
+      <c r="U191">
+        <v>2.8233450000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>